<commit_message>
Windows Generic Credential Functionality Added
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5452734-3F2D-499D-96BA-99B5D70C519A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -49,9 +48,6 @@
     <t>Timeout</t>
   </si>
   <si>
-    <t>https://site020-ck3mqp9a.chartwire.com/mobiledoc/jsp/webemr/login/newLogin.jsp</t>
-  </si>
-  <si>
     <t>Common Delay(1000 = 1 sec) before time out exception</t>
   </si>
   <si>
@@ -64,9 +60,6 @@
     <t>Alphabets which needs to be searched for should be saparated by Comma</t>
   </si>
   <si>
-    <t>n,p</t>
-  </si>
-  <si>
     <t>Fresh_Run</t>
   </si>
   <si>
@@ -89,12 +82,18 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>https://masmdvapp.eclinicalweb.com/mobiledoc/jsp/webemr/login/newLogin.jsp</t>
+  </si>
+  <si>
+    <t>ab,ac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,11 +420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +450,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -462,7 +461,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -487,48 +486,48 @@
         <v>60000</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>